<commit_message>
numba is ready -- now we have to see if we gain any perfomance
</commit_message>
<xml_diff>
--- a/differential_privacy_logistic_regression/output.xlsx
+++ b/differential_privacy_logistic_regression/output.xlsx
@@ -18,9 +18,6 @@
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="10">
   <si>
     <t>N</t>
-  </si>
-  <si>
-    <t>Weights</t>
   </si>
   <si>
     <t>$\epsilon = 0.0005$</t>
@@ -45,6 +42,9 @@
   </si>
   <si>
     <t>$\epsilon = 3$</t>
+  </si>
+  <si>
+    <t>Weights</t>
   </si>
 </sst>
 </file>
@@ -448,31 +448,31 @@
         <v>21</v>
       </c>
       <c r="C2">
-        <v>0.06493964197984495</v>
+        <v>158.0688278697604</v>
       </c>
       <c r="D2">
-        <v>158.0478863823158</v>
+        <v>79.05336545289872</v>
       </c>
       <c r="E2">
-        <v>79.05266915150023</v>
+        <v>15.77442546854861</v>
       </c>
       <c r="F2">
-        <v>15.78625049087047</v>
+        <v>7.911110477161534</v>
       </c>
       <c r="G2">
-        <v>7.892642495151868</v>
+        <v>1.579329682280626</v>
       </c>
       <c r="H2">
-        <v>1.580914283925423</v>
+        <v>0.7893463099091917</v>
       </c>
       <c r="I2">
-        <v>0.7901451722324775</v>
+        <v>0.1578901368217719</v>
       </c>
       <c r="J2">
-        <v>0.1578056334464977</v>
+        <v>0.02629573490310636</v>
       </c>
       <c r="K2">
-        <v>0.02638179709343885</v>
+        <v>0.001637830735344022</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -483,31 +483,31 @@
         <v>42</v>
       </c>
       <c r="C3">
-        <v>0.07026632359238848</v>
+        <v>157.9936466259097</v>
       </c>
       <c r="D3">
-        <v>158.0381057212473</v>
+        <v>78.86714290354189</v>
       </c>
       <c r="E3">
-        <v>79.03743055733159</v>
+        <v>15.84026788746038</v>
       </c>
       <c r="F3">
-        <v>15.82848226118638</v>
+        <v>7.896287163348887</v>
       </c>
       <c r="G3">
-        <v>7.894368566938582</v>
+        <v>1.578787305226836</v>
       </c>
       <c r="H3">
-        <v>1.579195677459108</v>
+        <v>0.7904772314427679</v>
       </c>
       <c r="I3">
-        <v>0.7883992896985323</v>
+        <v>0.1577971005734869</v>
       </c>
       <c r="J3">
-        <v>0.1581464218985131</v>
+        <v>0.02635086897430705</v>
       </c>
       <c r="K3">
-        <v>0.02634949544395256</v>
+        <v>0.001263670303085209</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -518,31 +518,31 @@
         <v>63</v>
       </c>
       <c r="C4">
-        <v>0.07437683105941731</v>
+        <v>158.0106332225969</v>
       </c>
       <c r="D4">
-        <v>157.9432928613431</v>
+        <v>79.1854257510394</v>
       </c>
       <c r="E4">
-        <v>78.92978514879294</v>
+        <v>15.8079945778298</v>
       </c>
       <c r="F4">
-        <v>15.7845989707426</v>
+        <v>7.909653176262839</v>
       </c>
       <c r="G4">
-        <v>7.897685638700452</v>
+        <v>1.575051601553223</v>
       </c>
       <c r="H4">
-        <v>1.580628286781461</v>
+        <v>0.788970150746177</v>
       </c>
       <c r="I4">
-        <v>0.791799693919417</v>
+        <v>0.1579068543628789</v>
       </c>
       <c r="J4">
-        <v>0.1581310228820975</v>
+        <v>0.02643033426596556</v>
       </c>
       <c r="K4">
-        <v>0.02634098780434938</v>
+        <v>0.00125661083996006</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -553,31 +553,31 @@
         <v>84</v>
       </c>
       <c r="C5">
-        <v>0.07883038441164858</v>
+        <v>157.8264703766389</v>
       </c>
       <c r="D5">
-        <v>157.7199959605953</v>
+        <v>79.11088157410612</v>
       </c>
       <c r="E5">
-        <v>79.02869691627335</v>
+        <v>15.75467045057052</v>
       </c>
       <c r="F5">
-        <v>15.82245258220062</v>
+        <v>7.899593005543904</v>
       </c>
       <c r="G5">
-        <v>7.899049843779007</v>
+        <v>1.580623648535944</v>
       </c>
       <c r="H5">
-        <v>1.578948002777905</v>
+        <v>0.7924772333903534</v>
       </c>
       <c r="I5">
-        <v>0.788523646246799</v>
+        <v>0.1583236368438386</v>
       </c>
       <c r="J5">
-        <v>0.1577166893976619</v>
+        <v>0.02631171628035118</v>
       </c>
       <c r="K5">
-        <v>0.02633702414767514</v>
+        <v>0.001172953421322764</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -588,31 +588,31 @@
         <v>105</v>
       </c>
       <c r="C6">
-        <v>0.08164655241389615</v>
+        <v>158.3703944047845</v>
       </c>
       <c r="D6">
-        <v>157.7484529069328</v>
+        <v>78.95949697530881</v>
       </c>
       <c r="E6">
-        <v>79.02395372185889</v>
+        <v>15.81737603425909</v>
       </c>
       <c r="F6">
-        <v>15.80245497149506</v>
+        <v>7.907589818270206</v>
       </c>
       <c r="G6">
-        <v>7.887479961726769</v>
+        <v>1.581647538379609</v>
       </c>
       <c r="H6">
-        <v>1.579244311290112</v>
+        <v>0.7914178172239767</v>
       </c>
       <c r="I6">
-        <v>0.7931980843714409</v>
+        <v>0.1581269137705753</v>
       </c>
       <c r="J6">
-        <v>0.1580892077810346</v>
+        <v>0.02634953162634622</v>
       </c>
       <c r="K6">
-        <v>0.02636944073367135</v>
+        <v>0.0004758824762643964</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -623,31 +623,31 @@
         <v>126</v>
       </c>
       <c r="C7">
-        <v>0.04050193562582065</v>
+        <v>157.819168518465</v>
       </c>
       <c r="D7">
-        <v>157.8613149604426</v>
+        <v>79.03703695391792</v>
       </c>
       <c r="E7">
-        <v>79.24631748959331</v>
+        <v>15.81620235133372</v>
       </c>
       <c r="F7">
-        <v>15.79750911990418</v>
+        <v>7.907834739957322</v>
       </c>
       <c r="G7">
-        <v>7.89536562058508</v>
+        <v>1.581445677609782</v>
       </c>
       <c r="H7">
-        <v>1.579356452993595</v>
+        <v>0.7898172878621201</v>
       </c>
       <c r="I7">
-        <v>0.7913077637235835</v>
+        <v>0.1581725699100923</v>
       </c>
       <c r="J7">
-        <v>0.1580024872045983</v>
+        <v>0.02636556072963221</v>
       </c>
       <c r="K7">
-        <v>0.02640412827643385</v>
+        <v>0.001283062887174413</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -658,31 +658,31 @@
         <v>147</v>
       </c>
       <c r="C8">
-        <v>0.08392280381045039</v>
+        <v>157.7064334926939</v>
       </c>
       <c r="D8">
-        <v>157.8658601675323</v>
+        <v>79.14275146460395</v>
       </c>
       <c r="E8">
-        <v>78.88239578303649</v>
+        <v>15.79859531894928</v>
       </c>
       <c r="F8">
-        <v>15.78835832454834</v>
+        <v>7.90817213552601</v>
       </c>
       <c r="G8">
-        <v>7.895914543197917</v>
+        <v>1.578255476177183</v>
       </c>
       <c r="H8">
-        <v>1.577390221471087</v>
+        <v>0.7897679477538857</v>
       </c>
       <c r="I8">
-        <v>0.7907975757055896</v>
+        <v>0.1577045552998541</v>
       </c>
       <c r="J8">
-        <v>0.1581407704291108</v>
+        <v>0.02634600115552062</v>
       </c>
       <c r="K8">
-        <v>0.02634566372005862</v>
+        <v>0.0002468555559240835</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -693,31 +693,31 @@
         <v>168</v>
       </c>
       <c r="C9">
-        <v>0.08529266366656631</v>
+        <v>158.077046910276</v>
       </c>
       <c r="D9">
-        <v>158.2368893197335</v>
+        <v>79.00182780034851</v>
       </c>
       <c r="E9">
-        <v>78.8931608886856</v>
+        <v>15.7893807605487</v>
       </c>
       <c r="F9">
-        <v>15.78572900779341</v>
+        <v>7.908362050662186</v>
       </c>
       <c r="G9">
-        <v>7.908623207601776</v>
+        <v>1.581679992131252</v>
       </c>
       <c r="H9">
-        <v>1.578094182650653</v>
+        <v>0.7887079040819422</v>
       </c>
       <c r="I9">
-        <v>0.7915610445913766</v>
+        <v>0.1582168938604664</v>
       </c>
       <c r="J9">
-        <v>0.1580036953849504</v>
+        <v>0.02631528379336331</v>
       </c>
       <c r="K9">
-        <v>0.02630713708115578</v>
+        <v>8.433435698692454e-05</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -728,31 +728,31 @@
         <v>189</v>
       </c>
       <c r="C10">
-        <v>0.0866747739397721</v>
+        <v>158.1648500454752</v>
       </c>
       <c r="D10">
-        <v>158.229989048095</v>
+        <v>78.96925490385999</v>
       </c>
       <c r="E10">
-        <v>79.01109021135807</v>
+        <v>15.81272143428852</v>
       </c>
       <c r="F10">
-        <v>15.80558536196595</v>
+        <v>7.914238040756166</v>
       </c>
       <c r="G10">
-        <v>7.885827989782633</v>
+        <v>1.581450900658315</v>
       </c>
       <c r="H10">
-        <v>1.583444714337284</v>
+        <v>0.790035367734804</v>
       </c>
       <c r="I10">
-        <v>0.7910957559711858</v>
+        <v>0.1582959028008062</v>
       </c>
       <c r="J10">
-        <v>0.1580171064062226</v>
+        <v>0.02630744535160921</v>
       </c>
       <c r="K10">
-        <v>0.02627666375494354</v>
+        <v>-0.000347389520512437</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -763,31 +763,31 @@
         <v>210</v>
       </c>
       <c r="C11">
-        <v>0.08912525229886485</v>
+        <v>158.2386448695727</v>
       </c>
       <c r="D11">
-        <v>158.0433218026607</v>
+        <v>78.80097424237991</v>
       </c>
       <c r="E11">
-        <v>78.91855886077404</v>
+        <v>15.80663277067362</v>
       </c>
       <c r="F11">
-        <v>15.82529818069846</v>
+        <v>7.908449611390294</v>
       </c>
       <c r="G11">
-        <v>7.892380268330761</v>
+        <v>1.581340383426711</v>
       </c>
       <c r="H11">
-        <v>1.583458211571336</v>
+        <v>0.7899110040838146</v>
       </c>
       <c r="I11">
-        <v>0.7914009834340877</v>
+        <v>0.1578444353889548</v>
       </c>
       <c r="J11">
-        <v>0.1580261706127219</v>
+        <v>0.02630472123321671</v>
       </c>
       <c r="K11">
-        <v>0.02632339525460298</v>
+        <v>-0.0001551035771935032</v>
       </c>
     </row>
     <row r="12" spans="1:11">
@@ -798,31 +798,31 @@
         <v>231</v>
       </c>
       <c r="C12">
-        <v>0.08942417819746092</v>
+        <v>158.0621574291321</v>
       </c>
       <c r="D12">
-        <v>157.939491535741</v>
+        <v>79.16050449892978</v>
       </c>
       <c r="E12">
-        <v>79.05144896038516</v>
+        <v>15.79237389519561</v>
       </c>
       <c r="F12">
-        <v>15.80467158212577</v>
+        <v>7.917799444688045</v>
       </c>
       <c r="G12">
-        <v>7.90513622229633</v>
+        <v>1.579782560716009</v>
       </c>
       <c r="H12">
-        <v>1.578015270630922</v>
+        <v>0.7906671902218425</v>
       </c>
       <c r="I12">
-        <v>0.7890016234468458</v>
+        <v>0.1583295872741402</v>
       </c>
       <c r="J12">
-        <v>0.1580460781762743</v>
+        <v>0.02636122437006319</v>
       </c>
       <c r="K12">
-        <v>0.02633218102412132</v>
+        <v>-0.0001906093313675458</v>
       </c>
     </row>
     <row r="13" spans="1:11">
@@ -833,31 +833,31 @@
         <v>252</v>
       </c>
       <c r="C13">
-        <v>0.0907981458379595</v>
+        <v>158.0987054313068</v>
       </c>
       <c r="D13">
-        <v>158.1592339130556</v>
+        <v>78.90388884650565</v>
       </c>
       <c r="E13">
-        <v>78.96600409149254</v>
+        <v>15.77671768711285</v>
       </c>
       <c r="F13">
-        <v>15.77336865581373</v>
+        <v>7.925496359190459</v>
       </c>
       <c r="G13">
-        <v>7.909407350078101</v>
+        <v>1.577241241926728</v>
       </c>
       <c r="H13">
-        <v>1.581360966791908</v>
+        <v>0.7899001872789395</v>
       </c>
       <c r="I13">
-        <v>0.7908846326721398</v>
+        <v>0.1578590172426838</v>
       </c>
       <c r="J13">
-        <v>0.1579222566456767</v>
+        <v>0.02629645447558512</v>
       </c>
       <c r="K13">
-        <v>0.02634337216166907</v>
+        <v>-0.0005828888420591587</v>
       </c>
     </row>
     <row r="14" spans="1:11">
@@ -868,31 +868,31 @@
         <v>273</v>
       </c>
       <c r="C14">
-        <v>0.04861476391259662</v>
+        <v>157.9517182604025</v>
       </c>
       <c r="D14">
-        <v>157.8259560417397</v>
+        <v>78.84022008118109</v>
       </c>
       <c r="E14">
-        <v>79.08889112239895</v>
+        <v>15.77381847377514</v>
       </c>
       <c r="F14">
-        <v>15.82414924327984</v>
+        <v>7.900640635118423</v>
       </c>
       <c r="G14">
-        <v>7.904564000536927</v>
+        <v>1.580605594325018</v>
       </c>
       <c r="H14">
-        <v>1.58163225857711</v>
+        <v>0.7917953462130278</v>
       </c>
       <c r="I14">
-        <v>0.7916860622463419</v>
+        <v>0.1586813218178441</v>
       </c>
       <c r="J14">
-        <v>0.1580254417174481</v>
+        <v>0.02636423608493736</v>
       </c>
       <c r="K14">
-        <v>0.02633503078985995</v>
+        <v>0.00087430426807908</v>
       </c>
     </row>
     <row r="15" spans="1:11">
@@ -903,31 +903,31 @@
         <v>294</v>
       </c>
       <c r="C15">
-        <v>0.05700436926412182</v>
+        <v>157.7258953840803</v>
       </c>
       <c r="D15">
-        <v>158.3166101146706</v>
+        <v>78.88333445460057</v>
       </c>
       <c r="E15">
-        <v>79.10051613587335</v>
+        <v>15.84159065333031</v>
       </c>
       <c r="F15">
-        <v>15.80425654481049</v>
+        <v>7.907640730730147</v>
       </c>
       <c r="G15">
-        <v>7.888502119081279</v>
+        <v>1.579106709261391</v>
       </c>
       <c r="H15">
-        <v>1.578790787158165</v>
+        <v>0.7896644720224095</v>
       </c>
       <c r="I15">
-        <v>0.7914132370803041</v>
+        <v>0.1580550011812424</v>
       </c>
       <c r="J15">
-        <v>0.157971670330354</v>
+        <v>0.02634704698199194</v>
       </c>
       <c r="K15">
-        <v>0.02637871564230254</v>
+        <v>0.001627840560397385</v>
       </c>
     </row>
     <row r="16" spans="1:11">
@@ -938,31 +938,31 @@
         <v>315</v>
       </c>
       <c r="C16">
-        <v>0.06156291384674405</v>
+        <v>158.089302378476</v>
       </c>
       <c r="D16">
-        <v>157.5259829762751</v>
+        <v>79.06467286625221</v>
       </c>
       <c r="E16">
-        <v>79.0209386026018</v>
+        <v>15.81367262652027</v>
       </c>
       <c r="F16">
-        <v>15.79811630114727</v>
+        <v>7.911791930586967</v>
       </c>
       <c r="G16">
-        <v>7.910384622448243</v>
+        <v>1.582015793768093</v>
       </c>
       <c r="H16">
-        <v>1.577071076572786</v>
+        <v>0.7903568898610356</v>
       </c>
       <c r="I16">
-        <v>0.7901943375798736</v>
+        <v>0.1579501435514131</v>
       </c>
       <c r="J16">
-        <v>0.1579732270074192</v>
+        <v>0.02642692871810127</v>
       </c>
       <c r="K16">
-        <v>0.02635120445191112</v>
+        <v>0.00161531834432339</v>
       </c>
     </row>
   </sheetData>
@@ -1018,31 +1018,31 @@
         <v>21</v>
       </c>
       <c r="C2">
-        <v>0.00332356293672849</v>
+        <v>0.5388971139192631</v>
       </c>
       <c r="D2">
-        <v>0.3631817244152525</v>
+        <v>0.1664125465440106</v>
       </c>
       <c r="E2">
-        <v>0.0495520056272962</v>
+        <v>0.002182387485425093</v>
       </c>
       <c r="F2">
-        <v>0.002789362939024862</v>
+        <v>0.001503397383743446</v>
       </c>
       <c r="G2">
-        <v>0.0003694704933082908</v>
+        <v>1.634487692138122e-05</v>
       </c>
       <c r="H2">
-        <v>9.755753839738557e-06</v>
+        <v>1.011565171622803e-05</v>
       </c>
       <c r="I2">
-        <v>8.759081711405868e-06</v>
+        <v>5.882899279185047e-07</v>
       </c>
       <c r="J2">
-        <v>1.38739950438404e-07</v>
+        <v>6.396663408410638e-09</v>
       </c>
       <c r="K2">
-        <v>1.148387691892209e-08</v>
+        <v>0.003332138915318018</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -1053,31 +1053,31 @@
         <v>42</v>
       </c>
       <c r="C3">
-        <v>0.004125030198287277</v>
+        <v>0.3335323798321853</v>
       </c>
       <c r="D3">
-        <v>0.1049215862710887</v>
+        <v>0.03572147323037055</v>
       </c>
       <c r="E3">
-        <v>0.1055983348096631</v>
+        <v>0.002475247567155695</v>
       </c>
       <c r="F3">
-        <v>0.003152411307721839</v>
+        <v>0.0004035365706866905</v>
       </c>
       <c r="G3">
-        <v>0.001062925879978626</v>
+        <v>2.643348702667772e-05</v>
       </c>
       <c r="H3">
-        <v>1.010690363017067e-05</v>
+        <v>6.427989801974283e-06</v>
       </c>
       <c r="I3">
-        <v>3.994191302929812e-06</v>
+        <v>4.45252362129621e-07</v>
       </c>
       <c r="J3">
-        <v>1.334855687448003e-07</v>
+        <v>4.214114203172238e-09</v>
       </c>
       <c r="K3">
-        <v>5.540743837588645e-09</v>
+        <v>0.003767373189123533</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -1088,31 +1088,31 @@
         <v>63</v>
       </c>
       <c r="C4">
-        <v>0.004612874583820661</v>
+        <v>0.3008125773376262</v>
       </c>
       <c r="D4">
-        <v>0.2810274503408482</v>
+        <v>0.03514962242569448</v>
       </c>
       <c r="E4">
-        <v>0.09499996736244587</v>
+        <v>0.001876222959648762</v>
       </c>
       <c r="F4">
-        <v>0.002229521226325224</v>
+        <v>0.0005838257044296208</v>
       </c>
       <c r="G4">
-        <v>0.0005315159573738727</v>
+        <v>3.079697062622574e-05</v>
       </c>
       <c r="H4">
-        <v>2.440917764633442e-05</v>
+        <v>1.171617735211757e-05</v>
       </c>
       <c r="I4">
-        <v>4.015301900266976e-06</v>
+        <v>2.910251648569854e-07</v>
       </c>
       <c r="J4">
-        <v>2.200076191199737e-07</v>
+        <v>4.471074262604271e-09</v>
       </c>
       <c r="K4">
-        <v>7.702044751731628e-09</v>
+        <v>0.004404665111276523</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -1123,31 +1123,31 @@
         <v>84</v>
       </c>
       <c r="C5">
-        <v>0.005614770176577882</v>
+        <v>0.01932884489126172</v>
       </c>
       <c r="D5">
-        <v>0.2556796305220183</v>
+        <v>0.1006075961147395</v>
       </c>
       <c r="E5">
-        <v>0.04641733893495496</v>
+        <v>0.0038592891592249</v>
       </c>
       <c r="F5">
-        <v>0.004294231858691204</v>
+        <v>0.001455113291182925</v>
       </c>
       <c r="G5">
-        <v>0.0007566153466245658</v>
+        <v>1.554817879565704e-05</v>
       </c>
       <c r="H5">
-        <v>1.798369336444597e-05</v>
+        <v>1.269924375156924e-05</v>
       </c>
       <c r="I5">
-        <v>7.519084130465154e-06</v>
+        <v>4.247439195904293e-07</v>
       </c>
       <c r="J5">
-        <v>1.001614536082878e-07</v>
+        <v>1.211004136715657e-08</v>
       </c>
       <c r="K5">
-        <v>1.091811841497218e-08</v>
+        <v>0.004701543263375125</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -1158,31 +1158,31 @@
         <v>105</v>
       </c>
       <c r="C6">
-        <v>0.005967499105813306</v>
+        <v>0.1575168639765247</v>
       </c>
       <c r="D6">
-        <v>0.6599398142432044</v>
+        <v>0.240170097911845</v>
       </c>
       <c r="E6">
-        <v>0.0550830325923449</v>
+        <v>0.004476703788686597</v>
       </c>
       <c r="F6">
-        <v>0.003502450841054335</v>
+        <v>0.001206297079026628</v>
       </c>
       <c r="G6">
-        <v>0.0009220397106543109</v>
+        <v>9.719829027587821e-06</v>
       </c>
       <c r="H6">
-        <v>4.489194339091865e-05</v>
+        <v>1.170915032022572e-05</v>
       </c>
       <c r="I6">
-        <v>2.341695900904642e-05</v>
+        <v>2.424456167618441e-07</v>
       </c>
       <c r="J6">
-        <v>1.652711354487968e-07</v>
+        <v>8.950391493102031e-09</v>
       </c>
       <c r="K6">
-        <v>1.274181128887763e-08</v>
+        <v>0.005311560451219446</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -1193,31 +1193,31 @@
         <v>126</v>
       </c>
       <c r="C7">
-        <v>0.001305575715152199</v>
+        <v>0.1337965642494017</v>
       </c>
       <c r="D7">
-        <v>0.5324529815134649</v>
+        <v>0.07880443229547093</v>
       </c>
       <c r="E7">
-        <v>0.04795509673426378</v>
+        <v>0.002355992711585806</v>
       </c>
       <c r="F7">
-        <v>0.004285121932804148</v>
+        <v>0.0008650009184373336</v>
       </c>
       <c r="G7">
-        <v>0.00052729261524868</v>
+        <v>4.139375405241967e-05</v>
       </c>
       <c r="H7">
-        <v>5.073036505373365e-06</v>
+        <v>4.856204543240151e-06</v>
       </c>
       <c r="I7">
-        <v>8.913604239604418e-06</v>
+        <v>2.428254368799974e-07</v>
       </c>
       <c r="J7">
-        <v>1.072697405927225e-07</v>
+        <v>6.895632761711884e-09</v>
       </c>
       <c r="K7">
-        <v>6.459123596333199e-09</v>
+        <v>0.001258530223895063</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -1228,31 +1228,31 @@
         <v>147</v>
       </c>
       <c r="C8">
-        <v>0.006668662516689466</v>
+        <v>0.5160521199099239</v>
       </c>
       <c r="D8">
-        <v>0.1378735140142188</v>
+        <v>0.1050571029393607</v>
       </c>
       <c r="E8">
-        <v>0.06763629182733441</v>
+        <v>0.00390920208018836</v>
       </c>
       <c r="F8">
-        <v>0.007071743413584083</v>
+        <v>0.000635778347066127</v>
       </c>
       <c r="G8">
-        <v>0.001256050049831919</v>
+        <v>4.883158279649392e-06</v>
       </c>
       <c r="H8">
-        <v>2.19452395089188e-05</v>
+        <v>6.357338445237126e-06</v>
       </c>
       <c r="I8">
-        <v>1.20267943226872e-05</v>
+        <v>2.364545991994919e-07</v>
       </c>
       <c r="J8">
-        <v>1.538204239664775e-07</v>
+        <v>7.323844590964111e-09</v>
       </c>
       <c r="K8">
-        <v>1.145457045870533e-08</v>
+        <v>0.005670030180593685</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -1263,31 +1263,31 @@
         <v>168</v>
       </c>
       <c r="C9">
-        <v>0.00735509700617561</v>
+        <v>0.08004406598556439</v>
       </c>
       <c r="D9">
-        <v>0.1996471712465956</v>
+        <v>0.1130714190438923</v>
       </c>
       <c r="E9">
-        <v>0.1522714001808407</v>
+        <v>0.00509915606076483</v>
       </c>
       <c r="F9">
-        <v>0.004160928204152679</v>
+        <v>0.001665191674019315</v>
       </c>
       <c r="G9">
-        <v>0.0009425909815111857</v>
+        <v>1.692227814074824e-05</v>
       </c>
       <c r="H9">
-        <v>3.37883913497786e-05</v>
+        <v>1.006790094344584e-05</v>
       </c>
       <c r="I9">
-        <v>4.185406747673185e-06</v>
+        <v>3.121669004591994e-07</v>
       </c>
       <c r="J9">
-        <v>6.775699733951111e-07</v>
+        <v>1.055792321325364e-08</v>
       </c>
       <c r="K9">
-        <v>1.554286627161078e-08</v>
+        <v>0.005781157698736042</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -1298,31 +1298,31 @@
         <v>189</v>
       </c>
       <c r="C10">
-        <v>0.00763077551099897</v>
+        <v>0.710564794046785</v>
       </c>
       <c r="D10">
-        <v>0.5020078221700345</v>
+        <v>0.07238609733290943</v>
       </c>
       <c r="E10">
-        <v>0.1029818972920855</v>
+        <v>0.004281897183314638</v>
       </c>
       <c r="F10">
-        <v>0.002989298514465612</v>
+        <v>0.0007026731990371843</v>
       </c>
       <c r="G10">
-        <v>0.0003946081549944809</v>
+        <v>5.554532040487149e-05</v>
       </c>
       <c r="H10">
-        <v>4.781016201618641e-05</v>
+        <v>6.947884146959398e-06</v>
       </c>
       <c r="I10">
-        <v>6.888562348648614e-06</v>
+        <v>5.999492166946845e-07</v>
       </c>
       <c r="J10">
-        <v>4.946407277823065e-07</v>
+        <v>9.577691802518973e-09</v>
       </c>
       <c r="K10">
-        <v>4.790587671010673e-09</v>
+        <v>0.006049668660252355</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -1333,31 +1333,31 @@
         <v>210</v>
       </c>
       <c r="C11">
-        <v>0.008296587958031277</v>
+        <v>0.07546626211931667</v>
       </c>
       <c r="D11">
-        <v>0.1668586410049314</v>
+        <v>0.03105487268236645</v>
       </c>
       <c r="E11">
-        <v>0.138399777953869</v>
+        <v>0.002282794550209682</v>
       </c>
       <c r="F11">
-        <v>0.003377619888325739</v>
+        <v>0.001335590122854807</v>
       </c>
       <c r="G11">
-        <v>0.0009525792427089034</v>
+        <v>2.226516105539521e-05</v>
       </c>
       <c r="H11">
-        <v>2.623202942227931e-05</v>
+        <v>6.254092754772214e-06</v>
       </c>
       <c r="I11">
-        <v>6.587576091056378e-06</v>
+        <v>6.222764334533833e-07</v>
       </c>
       <c r="J11">
-        <v>2.363048715205182e-07</v>
+        <v>1.929645180875972e-09</v>
       </c>
       <c r="K11">
-        <v>4.779201757998516e-09</v>
+        <v>0.006300797354183731</v>
       </c>
     </row>
     <row r="12" spans="1:11">
@@ -1368,31 +1368,31 @@
         <v>231</v>
       </c>
       <c r="C12">
-        <v>0.008422322834654454</v>
+        <v>0.3259830440040595</v>
       </c>
       <c r="D12">
-        <v>0.4943224226036498</v>
+        <v>0.09396517814153946</v>
       </c>
       <c r="E12">
-        <v>0.1053470928973504</v>
+        <v>0.003993786168457676</v>
       </c>
       <c r="F12">
-        <v>0.001611950866471956</v>
+        <v>0.002559544451310559</v>
       </c>
       <c r="G12">
-        <v>0.0007079463744345223</v>
+        <v>1.919523306323559e-05</v>
       </c>
       <c r="H12">
-        <v>2.375754876669632e-05</v>
+        <v>2.740140281862689e-05</v>
       </c>
       <c r="I12">
-        <v>1.36708061437566e-05</v>
+        <v>1.488700388683028e-07</v>
       </c>
       <c r="J12">
-        <v>2.478331771448163e-07</v>
+        <v>1.514753493006979e-08</v>
       </c>
       <c r="K12">
-        <v>1.474971177023698e-08</v>
+        <v>0.006499712033847863</v>
       </c>
     </row>
     <row r="13" spans="1:11">
@@ -1403,31 +1403,31 @@
         <v>252</v>
       </c>
       <c r="C13">
-        <v>0.00880668620142331</v>
+        <v>0.2246792436929469</v>
       </c>
       <c r="D13">
-        <v>0.4720303420855072</v>
+        <v>0.0939191814506338</v>
       </c>
       <c r="E13">
-        <v>0.2327252713845736</v>
+        <v>0.001355182031456266</v>
       </c>
       <c r="F13">
-        <v>0.004007600764519464</v>
+        <v>0.0003458398931492565</v>
       </c>
       <c r="G13">
-        <v>0.0008335819465470971</v>
+        <v>2.749801794867621e-05</v>
       </c>
       <c r="H13">
-        <v>6.160573880994407e-06</v>
+        <v>1.231391417578391e-05</v>
       </c>
       <c r="I13">
-        <v>8.009904634427463e-06</v>
+        <v>1.920299593956377e-07</v>
       </c>
       <c r="J13">
-        <v>2.160058894032596e-07</v>
+        <v>1.328687565981286e-08</v>
       </c>
       <c r="K13">
-        <v>4.906847943340224e-09</v>
+        <v>0.006870055417105785</v>
       </c>
     </row>
     <row r="14" spans="1:11">
@@ -1438,31 +1438,31 @@
         <v>273</v>
       </c>
       <c r="C14">
-        <v>0.002064421131930338</v>
+        <v>0.3056032949815163</v>
       </c>
       <c r="D14">
-        <v>0.6385091294560007</v>
+        <v>0.03714426831907866</v>
       </c>
       <c r="E14">
-        <v>0.1263491404007507</v>
+        <v>0.006883794923718129</v>
       </c>
       <c r="F14">
-        <v>0.00278396101727092</v>
+        <v>0.0006258660675599264</v>
       </c>
       <c r="G14">
-        <v>0.001883106597168878</v>
+        <v>7.818105843218028e-05</v>
       </c>
       <c r="H14">
-        <v>9.878120908706154e-06</v>
+        <v>9.675663969027826e-06</v>
       </c>
       <c r="I14">
-        <v>2.359284299825803e-06</v>
+        <v>3.119007846344517e-07</v>
       </c>
       <c r="J14">
-        <v>4.067760990968982e-07</v>
+        <v>1.236937274783853e-08</v>
       </c>
       <c r="K14">
-        <v>2.188903539936854e-10</v>
+        <v>0.001984140473647917</v>
       </c>
     </row>
     <row r="15" spans="1:11">
@@ -1473,31 +1473,31 @@
         <v>294</v>
       </c>
       <c r="C15">
-        <v>0.002436187039919447</v>
+        <v>0.256661068438039</v>
       </c>
       <c r="D15">
-        <v>0.4969306676401298</v>
+        <v>0.1344784169910012</v>
       </c>
       <c r="E15">
-        <v>0.08689525238160677</v>
+        <v>0.00458523391110811</v>
       </c>
       <c r="F15">
-        <v>0.003061881166319017</v>
+        <v>0.0003324442987628269</v>
       </c>
       <c r="G15">
-        <v>0.0008183068550625</v>
+        <v>3.676226086865599e-05</v>
       </c>
       <c r="H15">
-        <v>1.251442518540501e-05</v>
+        <v>1.019010566417569e-05</v>
       </c>
       <c r="I15">
-        <v>4.422194397432551e-06</v>
+        <v>1.23503459029077e-07</v>
       </c>
       <c r="J15">
-        <v>2.584753917414728e-07</v>
+        <v>1.674979616051067e-08</v>
       </c>
       <c r="K15">
-        <v>7.633053858812995e-09</v>
+        <v>0.002403459947195086</v>
       </c>
     </row>
     <row r="16" spans="1:11">
@@ -1508,31 +1508,31 @@
         <v>315</v>
       </c>
       <c r="C16">
-        <v>0.002912780034711734</v>
+        <v>0.1142274935728161</v>
       </c>
       <c r="D16">
-        <v>0.35871070661203</v>
+        <v>0.05448332624284676</v>
       </c>
       <c r="E16">
-        <v>0.09997235570296925</v>
+        <v>0.0029566651686651</v>
       </c>
       <c r="F16">
-        <v>0.005791721513624091</v>
+        <v>0.0003877569262783366</v>
       </c>
       <c r="G16">
-        <v>0.00162294771134269</v>
+        <v>2.717115401400796e-05</v>
       </c>
       <c r="H16">
-        <v>1.051036773653128e-05</v>
+        <v>1.33918030892793e-05</v>
       </c>
       <c r="I16">
-        <v>5.348578601444704e-06</v>
+        <v>5.822055549523775e-07</v>
       </c>
       <c r="J16">
-        <v>1.487637892282445e-07</v>
+        <v>4.537186840774366e-09</v>
       </c>
       <c r="K16">
-        <v>1.134405300933329e-08</v>
+        <v>0.002859514089584859</v>
       </c>
     </row>
   </sheetData>

</xml_diff>